<commit_message>
Updated the MVN Repository for Test data from excel
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FTA_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50755A5D-398B-4475-BA44-E5A78597E44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9632C7AA-236B-4ADA-A8AA-6E0EC9C9E86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1C3122A5-E787-4F38-90D5-01C65E489592}"/>
   </bookViews>
@@ -239,10 +239,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -582,7 +582,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +608,7 @@
     <col min="19" max="19" width="14.7265625" customWidth="1"/>
     <col min="20" max="20" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.90625" customWidth="1"/>
-    <col min="22" max="22" width="22.81640625" customWidth="1"/>
+    <col min="22" max="22" width="26.08984375" customWidth="1"/>
     <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -751,11 +751,11 @@
       <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="5"/>
+      <c r="V2" s="6"/>
       <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="6"/>
+      <c r="X2" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Committed the create word document class
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FTA_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6396C9AF-5A9C-4B2D-A21E-DE7C33060221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E8DFC1-62DA-4FC5-AE20-65A05ECE6792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1C3122A5-E787-4F38-90D5-01C65E489592}"/>
   </bookViews>
@@ -226,13 +226,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,7 +571,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,13 +740,13 @@
       <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="4">
         <v>837</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new Add Address class and changes in existing classes
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FTA_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A81C51-B416-499A-A417-799993FE975C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F47543-A440-418F-A646-1612C649CB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1C3122A5-E787-4F38-90D5-01C65E489592}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>ModuleName</t>
   </si>
@@ -174,13 +174,109 @@
   </si>
   <si>
     <t>873</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Comapny_Name_ED</t>
+  </si>
+  <si>
+    <t>Country_ID_ED</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>City_ED</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>Address1_ED</t>
+  </si>
+  <si>
+    <t>Address2_ED</t>
+  </si>
+  <si>
+    <t>Gold mrket</t>
+  </si>
+  <si>
+    <t>ZipPostalCode_ED</t>
+  </si>
+  <si>
+    <t>PhoneNumber_ED</t>
+  </si>
+  <si>
+    <t>FaxNumber_ED</t>
+  </si>
+  <si>
+    <t>FieldValue11</t>
+  </si>
+  <si>
+    <t>FiledName11</t>
+  </si>
+  <si>
+    <t>FieldValue12</t>
+  </si>
+  <si>
+    <t>FiledName12</t>
+  </si>
+  <si>
+    <t>FieldValue13</t>
+  </si>
+  <si>
+    <t>FiledName13</t>
+  </si>
+  <si>
+    <t>FieldValue14</t>
+  </si>
+  <si>
+    <t>FiledName14</t>
+  </si>
+  <si>
+    <t>FieldValue15</t>
+  </si>
+  <si>
+    <t>FiledName15</t>
+  </si>
+  <si>
+    <t>FiledName16</t>
+  </si>
+  <si>
+    <t>FieldValu16</t>
+  </si>
+  <si>
+    <t>FiledName17</t>
+  </si>
+  <si>
+    <t>FieldValu17</t>
+  </si>
+  <si>
+    <t>401288888</t>
+  </si>
+  <si>
+    <t>40128888</t>
+  </si>
+  <si>
+    <t>40128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +288,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -233,10 +335,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB887A8-4189-4BC4-8B68-D6315F44F76E}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,9 +707,25 @@
     <col min="22" max="22" width="26.08984375" customWidth="1"/>
     <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.81640625" customWidth="1"/>
+    <col min="26" max="26" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.81640625" customWidth="1"/>
+    <col min="28" max="28" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.81640625" customWidth="1"/>
+    <col min="30" max="30" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.81640625" customWidth="1"/>
+    <col min="32" max="32" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.81640625" customWidth="1"/>
+    <col min="34" max="34" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.81640625" customWidth="1"/>
+    <col min="36" max="36" width="26.08984375" customWidth="1"/>
+    <col min="37" max="37" width="16.81640625" customWidth="1"/>
+    <col min="38" max="38" width="26.08984375" customWidth="1"/>
+    <col min="39" max="39" width="16.81640625" customWidth="1"/>
+    <col min="40" max="40" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +798,56 @@
       <c r="X1" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="Y1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -754,8 +920,290 @@
       <c r="X2" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="Z2" s="4"/>
+      <c r="AJ2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AN2" s="3"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="4"/>
+      <c r="AJ3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AN3" s="3"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AN4" s="3"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>